<commit_message>
Keynote titles and abstracts
</commit_message>
<xml_diff>
--- a/uRos2020_abstracts/abstracts.xlsx
+++ b/uRos2020_abstracts/abstracts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="351">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1356,6 +1356,42 @@
   </si>
   <si>
     <t>Wolfgang Rannetbauer</t>
+  </si>
+  <si>
+    <t>Isabel Molina Peralta</t>
+  </si>
+  <si>
+    <t>Universidad Carlos III de Madrid</t>
+  </si>
+  <si>
+    <t>Small area estimation using R, with application to poverty mapping.</t>
+  </si>
+  <si>
+    <t>Keynote</t>
+  </si>
+  <si>
+    <t>Small area estimation is a promising, but also well established and well developed family of methods to gain insights on detailed domains or areas. Not widely used in statistical offices yet, available resources in R provide an opportunity to change that. Existing R packages designed for small area estimation with a special focus on the applicability for poverty mapping are reviewed. Applications to poverty mapping are presented to illustrate some of the available functions.</t>
+  </si>
+  <si>
+    <t>Functional data analysis in Bayes Spaces with an Application to spatio-temporal population data</t>
+  </si>
+  <si>
+    <t>Matthias Templ</t>
+  </si>
+  <si>
+    <t>Probability density functions are frequently used to characterize the distributional properties of large-scale database systems. As functional compositions, densities carry primarily relative information. As such, standard methods of functional data analysis (FDA) are not appropriate for their statistical processing and thus a compositional alternative is proposed. The aim of this presentation is to outline a concise methodology for functional principal component analysis of densities based on the geometry of the Bayes space B2 of functional compositions. Advances of the proposed approach are demonstrated using a real-world example of population pyramids in Upper Austria. For compositional analysis we also introduce the R package robCompositions.</t>
+  </si>
+  <si>
+    <t>Kurt Hornik</t>
+  </si>
+  <si>
+    <t>Working with textual data ("text mining") is becoming increasingly important in modern statistics.  We show how R can be used for basic and advanced natural language processing tasks, manipulating collections of text documents, and deriving features/representations suitable for further statistical analyses.  We illustrate how these conceptual and computational tools can be employed in several applications, including document clustering, stylometry, cultoromics, semantic lexicon induction, extracting financial sentiment, and modeling readability.</t>
+  </si>
+  <si>
+    <t>Analyzing Texts with R</t>
+  </si>
+  <si>
+    <t>Zurich University of Applied Sciences</t>
   </si>
 </sst>
 </file>
@@ -1636,11 +1672,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q65"/>
+  <dimension ref="A1:Q68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I65" sqref="I65"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1648,7 +1684,7 @@
     <col min="1" max="23" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1701,7 +1737,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43867.339679594908</v>
       </c>
@@ -1724,7 +1760,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>43867.346029548615</v>
       </c>
@@ -1744,7 +1780,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>43867.347065324073</v>
       </c>
@@ -1779,7 +1815,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>43867.348353553243</v>
       </c>
@@ -1805,7 +1841,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>43867.349138634258</v>
       </c>
@@ -1825,7 +1861,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>43867.349999745369</v>
       </c>
@@ -1851,7 +1887,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>43867.350807592593</v>
       </c>
@@ -1874,7 +1910,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>43867.351438287034</v>
       </c>
@@ -1894,7 +1930,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>43867.352359675926</v>
       </c>
@@ -1923,7 +1959,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>43867.353283344906</v>
       </c>
@@ -1955,7 +1991,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>43867.353878437498</v>
       </c>
@@ -1975,7 +2011,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>43867.354641990736</v>
       </c>
@@ -1995,7 +2031,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>43867.355419189815</v>
       </c>
@@ -2018,7 +2054,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>43867.356136446761</v>
       </c>
@@ -2044,7 +2080,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>43867.357378275468</v>
       </c>
@@ -2064,7 +2100,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>43867.358166388891</v>
       </c>
@@ -2096,7 +2132,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43867.358798090281</v>
       </c>
@@ -2116,7 +2152,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>43867.359447557872</v>
       </c>
@@ -2136,7 +2172,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>43867.359879108801</v>
       </c>
@@ -2162,7 +2198,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>43867.360906759262</v>
       </c>
@@ -2188,7 +2224,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>43867.361841550926</v>
       </c>
@@ -2220,7 +2256,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>43867.363104687502</v>
       </c>
@@ -2261,7 +2297,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>43867.363585567131</v>
       </c>
@@ -2281,7 +2317,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>43867.364091053241</v>
       </c>
@@ -2301,7 +2337,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>43867.364760532408</v>
       </c>
@@ -2327,7 +2363,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>43867.365359143514</v>
       </c>
@@ -2347,7 +2383,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>43867.36666190972</v>
       </c>
@@ -2367,7 +2403,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>43867.367584953703</v>
       </c>
@@ -2393,7 +2429,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>43867.368431493058</v>
       </c>
@@ -2425,7 +2461,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>43867.36910974537</v>
       </c>
@@ -2448,7 +2484,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>43867.370430810188</v>
       </c>
@@ -2486,7 +2522,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>43867.371240555556</v>
       </c>
@@ -2512,7 +2548,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>43867.373401342593</v>
       </c>
@@ -2532,7 +2568,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>43867.374574629634</v>
       </c>
@@ -2564,7 +2600,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>43867.375863842593</v>
       </c>
@@ -2590,7 +2626,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>43867.376669606485</v>
       </c>
@@ -2625,7 +2661,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>43867.384836909725</v>
       </c>
@@ -2657,7 +2693,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>43867.386324143517</v>
       </c>
@@ -2695,7 +2731,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>43867.388082164354</v>
       </c>
@@ -2739,7 +2775,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>43867.389301504634</v>
       </c>
@@ -2777,7 +2813,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>43867.390828090276</v>
       </c>
@@ -2797,7 +2833,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>43867.392670648143</v>
       </c>
@@ -2835,7 +2871,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43867.39334008102</v>
       </c>
@@ -2867,7 +2903,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>43867.394623888889</v>
       </c>
@@ -2917,7 +2953,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>43867.395109687495</v>
       </c>
@@ -2937,7 +2973,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>43867.395944490738</v>
       </c>
@@ -2963,7 +2999,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>43867.396859872686</v>
       </c>
@@ -2986,7 +3022,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>43867.397601736113</v>
       </c>
@@ -3006,7 +3042,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>43867.398741689816</v>
       </c>
@@ -3044,7 +3080,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>43867.3994231713</v>
       </c>
@@ -3070,7 +3106,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>43867.399935231486</v>
       </c>
@@ -3090,7 +3126,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>43867.40033207176</v>
       </c>
@@ -3110,7 +3146,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>43867.401373923611</v>
       </c>
@@ -3130,7 +3166,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>43867.401838333331</v>
       </c>
@@ -3150,7 +3186,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>43867.402415937497</v>
       </c>
@@ -3173,7 +3209,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>43867.403161365743</v>
       </c>
@@ -3205,7 +3241,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>43867.403933310183</v>
       </c>
@@ -3237,7 +3273,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>43867.404456273143</v>
       </c>
@@ -3257,7 +3293,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>43867.405108391205</v>
       </c>
@@ -3283,7 +3319,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>43867.406668530093</v>
       </c>
@@ -3315,7 +3351,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>43867.40742974537</v>
       </c>
@@ -3347,7 +3383,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>43867.407841689812</v>
       </c>
@@ -3367,7 +3403,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>43867.414248842593</v>
       </c>
@@ -3411,6 +3447,66 @@
       </c>
       <c r="I65" s="5" t="s">
         <v>337</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2">
+        <v>43886.330914351849</v>
+      </c>
+      <c r="B66" t="s">
+        <v>341</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="F66" t="s">
+        <v>339</v>
+      </c>
+      <c r="G66" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2">
+        <v>43886.330914351849</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="2">
+        <v>43886.330914351849</v>
+      </c>
+      <c r="B68" t="s">
+        <v>349</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update affiliation (bifie -> iqs)
</commit_message>
<xml_diff>
--- a/uRos2020_abstracts/abstracts.xlsx
+++ b/uRos2020_abstracts/abstracts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\xwwp0017\profiles$\KOWA\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\xwwp0017\profiles$\meindl\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -916,9 +916,6 @@
     <t>Konrad Oberwimmer</t>
   </si>
   <si>
-    <t>BIFIE</t>
-  </si>
-  <si>
     <t>Integrated Weighting and Estimation System for Household Surveys with Complex Sampling Design</t>
   </si>
   <si>
@@ -1392,6 +1389,9 @@
   </si>
   <si>
     <t>Zurich University of Applied Sciences</t>
+  </si>
+  <si>
+    <t>IQS</t>
   </si>
 </sst>
 </file>
@@ -1675,8 +1675,8 @@
   <dimension ref="A1:Q68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2830,7 +2830,7 @@
         <v>222</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>223</v>
+        <v>350</v>
       </c>
     </row>
     <row r="43" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
@@ -2838,37 +2838,37 @@
         <v>43867.392670648143</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D43" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="G43" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="H43" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="H43" s="3" t="s">
+      <c r="I43" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="J43" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="I43" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="J43" s="3" t="s">
+      <c r="K43" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="L43" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="K43" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="L43" s="3" t="s">
+      <c r="M43" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="M43" s="3" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
@@ -2876,31 +2876,31 @@
         <v>43867.39334008102</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" s="3" t="s">
+      <c r="F44" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="G44" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="H44" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="H44" s="3" t="s">
+      <c r="I44" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="J44" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="I44" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="J44" s="3" t="s">
-        <v>237</v>
-      </c>
       <c r="K44" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
@@ -2908,46 +2908,46 @@
         <v>43867.394623888889</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>238</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>239</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>212</v>
       </c>
       <c r="G45" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="H45" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="H45" s="3" t="s">
+      <c r="I45" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="I45" s="3" t="s">
+      <c r="J45" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="J45" s="3" t="s">
+      <c r="K45" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="K45" s="3" t="s">
+      <c r="L45" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="L45" s="3" t="s">
+      <c r="M45" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="M45" s="3" t="s">
+      <c r="N45" s="3" t="s">
         <v>246</v>
-      </c>
-      <c r="N45" s="3" t="s">
-        <v>247</v>
       </c>
       <c r="O45" s="3" t="s">
         <v>213</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Q45" s="3" t="s">
         <v>213</v>
@@ -2958,19 +2958,19 @@
         <v>43867.395109687495</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D46" s="3" t="s">
+      <c r="F46" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="G46" s="3" t="s">
         <v>251</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
@@ -2978,22 +2978,22 @@
         <v>43867.395944490738</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D47" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>253</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>254</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>27</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I47" s="3" t="s">
         <v>27</v>
@@ -3004,22 +3004,22 @@
         <v>43867.396859872686</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D48" s="3" t="s">
+      <c r="E48" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="F48" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="G48" s="3" t="s">
         <v>259</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -3027,19 +3027,19 @@
         <v>43867.397601736113</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D49" s="3" t="s">
+      <c r="F49" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="G49" s="3" t="s">
         <v>263</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -3047,37 +3047,37 @@
         <v>43867.398741689816</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D50" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="F50" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="G50" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="G50" s="3" t="s">
+      <c r="H50" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="H50" s="3" t="s">
+      <c r="I50" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="J50" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="I50" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="J50" s="3" t="s">
+      <c r="K50" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="L50" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="K50" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="L50" s="3" t="s">
-        <v>271</v>
-      </c>
       <c r="M50" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -3085,25 +3085,25 @@
         <v>43867.3994231713</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D51" s="3" t="s">
+      <c r="F51" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="G51" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="G51" s="3" t="s">
+      <c r="H51" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="H51" s="3" t="s">
-        <v>276</v>
-      </c>
       <c r="I51" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -3111,19 +3111,19 @@
         <v>43867.399935231486</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D52" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="F52" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="G52" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -3131,19 +3131,19 @@
         <v>43867.40033207176</v>
       </c>
       <c r="B53" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>282</v>
-      </c>
       <c r="F53" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G53" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -3151,19 +3151,19 @@
         <v>43867.401373923611</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D54" s="3" t="s">
+      <c r="F54" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="G54" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -3171,19 +3171,19 @@
         <v>43867.401838333331</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -3191,22 +3191,22 @@
         <v>43867.402415937497</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D56" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="F56" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="G56" s="3" t="s">
         <v>293</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -3214,22 +3214,22 @@
         <v>43867.403161365743</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D57" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>296</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>297</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>57</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I57" s="3" t="s">
         <v>57</v>
@@ -3246,25 +3246,25 @@
         <v>43867.403933310183</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D58" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F58" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="F58" s="3" t="s">
+      <c r="G58" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="H58" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="G58" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>302</v>
-      </c>
       <c r="I58" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J58" s="3" t="s">
         <v>94</v>
@@ -3278,19 +3278,19 @@
         <v>43867.404456273143</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D59" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="F59" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="F59" s="3" t="s">
+      <c r="G59" s="3" t="s">
         <v>305</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -3298,25 +3298,25 @@
         <v>43867.405108391205</v>
       </c>
       <c r="B60" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D60" s="3" t="s">
+      <c r="F60" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="G60" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="G60" s="3" t="s">
+      <c r="H60" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="H60" s="3" t="s">
+      <c r="I60" s="3" t="s">
         <v>311</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -3324,31 +3324,31 @@
         <v>43867.406668530093</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D61" s="3" t="s">
+      <c r="F61" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="F61" s="3" t="s">
+      <c r="G61" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="G61" s="3" t="s">
+      <c r="H61" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="H61" s="3" t="s">
+      <c r="I61" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="J61" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="I61" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="J61" s="3" t="s">
-        <v>318</v>
-      </c>
       <c r="K61" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -3356,31 +3356,31 @@
         <v>43867.40742974537</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D62" s="3" t="s">
+      <c r="F62" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="G62" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="G62" s="3" t="s">
+      <c r="H62" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="H62" s="3" t="s">
+      <c r="I62" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="I62" s="3" t="s">
+      <c r="J62" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="J62" s="3" t="s">
+      <c r="K62" s="3" t="s">
         <v>325</v>
-      </c>
-      <c r="K62" s="3" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -3388,16 +3388,16 @@
         <v>43867.407841689812</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D63" s="3" t="s">
+      <c r="F63" s="3" t="s">
         <v>328</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>329</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>100</v>
@@ -3408,19 +3408,19 @@
         <v>43867.414248842593</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D64" s="3" t="s">
+      <c r="F64" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="F64" s="3" t="s">
-        <v>332</v>
-      </c>
       <c r="G64" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3428,25 +3428,25 @@
         <v>43885.330914351849</v>
       </c>
       <c r="B65" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D65" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="F65" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="F65" s="5" t="s">
+      <c r="G65" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="G65" s="5" t="s">
+      <c r="H65" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="H65" s="5" t="s">
-        <v>338</v>
-      </c>
       <c r="I65" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3454,19 +3454,19 @@
         <v>43886.330914351849</v>
       </c>
       <c r="B66" t="s">
+        <v>340</v>
+      </c>
+      <c r="C66" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="D66" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="D66" s="5" t="s">
-        <v>343</v>
-      </c>
       <c r="F66" t="s">
+        <v>338</v>
+      </c>
+      <c r="G66" t="s">
         <v>339</v>
-      </c>
-      <c r="G66" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3474,19 +3474,19 @@
         <v>43886.330914351849</v>
       </c>
       <c r="B67" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="F67" s="5" t="s">
         <v>344</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>345</v>
-      </c>
       <c r="G67" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3494,16 +3494,16 @@
         <v>43886.330914351849</v>
       </c>
       <c r="B68" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>22</v>

</xml_diff>